<commit_message>
change for README file
</commit_message>
<xml_diff>
--- a/task2/degree_distribution_data.xlsx
+++ b/task2/degree_distribution_data.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,15 +45,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -439,20 +439,20 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -460,47 +460,47 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>2145</v>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>4186</v>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>4560</v>
       </c>
       <c r="B8" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>4950</v>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>5151</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
@@ -508,14 +508,14 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>134421</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -525,7 +525,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -550,12 +550,12 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -563,15 +563,15 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -579,85 +579,37 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>2701</v>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>5565</v>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>361675</v>
       </c>
       <c r="B9" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed the each state as individual different cell
</commit_message>
<xml_diff>
--- a/task2/degree_distribution_data.xlsx
+++ b/task2/degree_distribution_data.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,74 +444,66 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>55</v>
+        <v>141</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2145</v>
+        <v>142</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4186</v>
+        <v>145</v>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4560</v>
+        <v>155</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4950</v>
+        <v>159</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5151</v>
+        <v>160</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>134421</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -525,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -550,63 +542,87 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
         <v>3</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>90</v>
+      </c>
+      <c r="B6" t="n">
         <v>91</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2701</v>
+        <v>140</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5565</v>
+        <v>152</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>361675</v>
+        <v>154</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>159</v>
+      </c>
+      <c r="B10" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>163</v>
+      </c>
+      <c r="B11" t="n">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>181</v>
+      </c>
+      <c r="B12" t="n">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>